<commit_message>
Updates - number box for scrolling rows/columns
</commit_message>
<xml_diff>
--- a/Poll_filechange/mySheet.xlsx
+++ b/Poll_filechange/mySheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="1820" windowWidth="23540" windowHeight="13200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Term</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>ABC transporters</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>Acute myeloid leukemia</t>
@@ -460,7 +457,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -506,11 +503,11 @@
       <c r="B3" s="1">
         <v>2010</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -518,7 +515,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>5221</v>
@@ -535,7 +532,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>4520</v>
@@ -552,7 +549,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>4920</v>
@@ -569,7 +566,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <v>5143</v>
@@ -586,7 +583,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1">
         <v>250</v>
@@ -603,7 +600,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1">
         <v>5034</v>
@@ -620,7 +617,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1">
         <v>4960</v>

</xml_diff>